<commit_message>
after hosting change 9
</commit_message>
<xml_diff>
--- a/controller/salesData.xlsx
+++ b/controller/salesData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="52">
   <si>
     <t>Order ID</t>
   </si>
@@ -134,6 +134,39 @@
   </si>
   <si>
     <t>955741</t>
+  </si>
+  <si>
+    <t>583986</t>
+  </si>
+  <si>
+    <t>654506</t>
+  </si>
+  <si>
+    <t>482437</t>
+  </si>
+  <si>
+    <t>602514</t>
+  </si>
+  <si>
+    <t>350675</t>
+  </si>
+  <si>
+    <t>964771</t>
+  </si>
+  <si>
+    <t>414660</t>
+  </si>
+  <si>
+    <t>454571</t>
+  </si>
+  <si>
+    <t>104689</t>
+  </si>
+  <si>
+    <t>269614</t>
+  </si>
+  <si>
+    <t>835677</t>
   </si>
 </sst>
 </file>
@@ -520,7 +553,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K57"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="11" width="30" style="1" customWidth="1"/>
@@ -561,372 +594,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1750</v>
-      </c>
-      <c r="G19" s="1">
-        <v>5250</v>
-      </c>
-      <c r="H19" s="3">
-        <v>45230.37326881944</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1">
-        <v>9000</v>
-      </c>
-      <c r="H20" s="3">
-        <v>45230.37413140046</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1">
-        <v>16000</v>
-      </c>
-      <c r="H21" s="3">
-        <v>45230.48288606481</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0</v>
-      </c>
-      <c r="G22" s="1">
-        <v>7000</v>
-      </c>
-      <c r="H22" s="3">
-        <v>45230.48312577546</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="1">
-        <v>3500</v>
-      </c>
-      <c r="G23" s="1">
-        <v>10500</v>
-      </c>
-      <c r="H23" s="3">
-        <v>45230.51429846065</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="1">
-        <v>0</v>
-      </c>
-      <c r="G24" s="1">
-        <v>7500</v>
-      </c>
-      <c r="H24" s="3">
-        <v>45230.51480040509</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25" s="1">
-        <v>0</v>
-      </c>
-      <c r="G25" s="1">
-        <v>7500</v>
-      </c>
-      <c r="H25" s="3">
-        <v>45230.51493697916</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" s="1">
-        <v>1750</v>
-      </c>
-      <c r="G26" s="1">
-        <v>5250</v>
-      </c>
-      <c r="H26" s="3">
-        <v>45230.517359826394</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="1">
-        <v>1875</v>
-      </c>
-      <c r="G27" s="1">
-        <v>5625</v>
-      </c>
-      <c r="H27" s="3">
-        <v>45230.526474178245</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="1">
-        <v>0</v>
-      </c>
-      <c r="G28" s="1">
-        <v>9000</v>
-      </c>
-      <c r="H28" s="3">
-        <v>45230.527110069444</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F29" s="1">
-        <v>0</v>
-      </c>
-      <c r="G29" s="1">
-        <v>7000</v>
-      </c>
-      <c r="H29" s="3">
-        <v>45230.545366770835</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="1">
-        <v>0</v>
-      </c>
-      <c r="G30" s="1">
-        <v>7000</v>
-      </c>
-      <c r="H30" s="3">
-        <v>45230.556492442134</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="F31" s="1">
-        <v>2250</v>
+        <v>1750</v>
       </c>
       <c r="G31" s="1">
-        <v>6750</v>
+        <v>5250</v>
       </c>
       <c r="H31" s="3">
-        <v>45230.56057988426</v>
+        <v>45230.37326881944</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>13</v>
@@ -940,36 +625,36 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="F32" s="1">
-        <v>1875</v>
+        <v>0</v>
       </c>
       <c r="G32" s="1">
-        <v>5625</v>
+        <v>9000</v>
       </c>
       <c r="H32" s="3">
-        <v>45230.575472627315</v>
+        <v>45230.37413140046</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -981,24 +666,24 @@
         <v>0</v>
       </c>
       <c r="G33" s="1">
-        <v>14000</v>
+        <v>16000</v>
       </c>
       <c r="H33" s="3">
-        <v>45231.41486247686</v>
+        <v>45230.48288606481</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1010,10 +695,10 @@
         <v>0</v>
       </c>
       <c r="G34" s="1">
-        <v>7500</v>
+        <v>7000</v>
       </c>
       <c r="H34" s="3">
-        <v>45231.41499884259</v>
+        <v>45230.48312577546</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>13</v>
@@ -1023,6 +708,673 @@
       </c>
       <c r="K34" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="1">
+        <v>3500</v>
+      </c>
+      <c r="G35" s="1">
+        <v>10500</v>
+      </c>
+      <c r="H35" s="3">
+        <v>45230.51429846065</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>7500</v>
+      </c>
+      <c r="H36" s="3">
+        <v>45230.51480040509</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>7500</v>
+      </c>
+      <c r="H37" s="3">
+        <v>45230.51493697916</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1750</v>
+      </c>
+      <c r="G38" s="1">
+        <v>5250</v>
+      </c>
+      <c r="H38" s="3">
+        <v>45230.517359826394</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1875</v>
+      </c>
+      <c r="G39" s="1">
+        <v>5625</v>
+      </c>
+      <c r="H39" s="3">
+        <v>45230.526474178245</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
+      <c r="G40" s="1">
+        <v>9000</v>
+      </c>
+      <c r="H40" s="3">
+        <v>45230.527110069444</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1">
+        <v>7000</v>
+      </c>
+      <c r="H41" s="3">
+        <v>45230.545366770835</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
+        <v>7000</v>
+      </c>
+      <c r="H42" s="3">
+        <v>45230.556492442134</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2250</v>
+      </c>
+      <c r="G43" s="1">
+        <v>6750</v>
+      </c>
+      <c r="H43" s="3">
+        <v>45230.56057988426</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1875</v>
+      </c>
+      <c r="G44" s="1">
+        <v>5625</v>
+      </c>
+      <c r="H44" s="3">
+        <v>45230.575472627315</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
+      <c r="G45" s="1">
+        <v>14000</v>
+      </c>
+      <c r="H45" s="3">
+        <v>45231.41486247686</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
+      <c r="G46" s="1">
+        <v>7500</v>
+      </c>
+      <c r="H46" s="3">
+        <v>45231.41499884259</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F47" s="1">
+        <v>2250</v>
+      </c>
+      <c r="G47" s="1">
+        <v>6750</v>
+      </c>
+      <c r="H47" s="3">
+        <v>45231.75643605324</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+      <c r="G48" s="1">
+        <v>16000</v>
+      </c>
+      <c r="H48" s="3">
+        <v>45231.765910428236</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+      <c r="G49" s="1">
+        <v>7000</v>
+      </c>
+      <c r="H49" s="3">
+        <v>45232.25594048611</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0</v>
+      </c>
+      <c r="G50" s="1">
+        <v>7500</v>
+      </c>
+      <c r="H50" s="3">
+        <v>45232.256089849536</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
+      <c r="G51" s="1">
+        <v>9000</v>
+      </c>
+      <c r="H51" s="3">
+        <v>45232.2562494213</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>7000</v>
+      </c>
+      <c r="H52" s="3">
+        <v>45232.25644429398</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+      <c r="G53" s="1">
+        <v>10500</v>
+      </c>
+      <c r="H53" s="3">
+        <v>45232.256622326386</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0</v>
+      </c>
+      <c r="G54" s="1">
+        <v>10500</v>
+      </c>
+      <c r="H54" s="3">
+        <v>45232.25677541667</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1">
+        <v>9000</v>
+      </c>
+      <c r="H55" s="3">
+        <v>45232.26625045139</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1">
+        <v>36000</v>
+      </c>
+      <c r="H56" s="3">
+        <v>45232.266521377314</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>234000</v>
+      </c>
+      <c r="H57" s="3">
+        <v>45232.26717273148</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
after hosting week review
</commit_message>
<xml_diff>
--- a/controller/salesData.xlsx
+++ b/controller/salesData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="54">
   <si>
     <t>Order ID</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>835677</t>
+  </si>
+  <si>
+    <t>618667</t>
+  </si>
+  <si>
+    <t>783506</t>
   </si>
 </sst>
 </file>
@@ -553,7 +559,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:K61"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="11" width="30" style="1" customWidth="1"/>
@@ -594,67 +600,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="1">
-        <v>1750</v>
-      </c>
-      <c r="G31" s="1">
-        <v>5250</v>
-      </c>
-      <c r="H31" s="3">
-        <v>45230.37326881944</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="1">
-        <v>0</v>
-      </c>
-      <c r="G32" s="1">
-        <v>9000</v>
-      </c>
-      <c r="H32" s="3">
-        <v>45230.37413140046</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -663,27 +611,27 @@
         <v>12</v>
       </c>
       <c r="F33" s="1">
-        <v>0</v>
+        <v>1750</v>
       </c>
       <c r="G33" s="1">
-        <v>16000</v>
+        <v>5250</v>
       </c>
       <c r="H33" s="3">
-        <v>45230.48288606481</v>
+        <v>45230.37326881944</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -695,82 +643,82 @@
         <v>0</v>
       </c>
       <c r="G34" s="1">
-        <v>7000</v>
+        <v>9000</v>
       </c>
       <c r="H34" s="3">
-        <v>45230.48312577546</v>
+        <v>45230.37413140046</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F35" s="1">
-        <v>3500</v>
+        <v>0</v>
       </c>
       <c r="G35" s="1">
-        <v>10500</v>
+        <v>16000</v>
       </c>
       <c r="H35" s="3">
-        <v>45230.51429846065</v>
+        <v>45230.48288606481</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F36" s="1">
         <v>0</v>
       </c>
       <c r="G36" s="1">
-        <v>7500</v>
+        <v>7000</v>
       </c>
       <c r="H36" s="3">
-        <v>45230.51480040509</v>
+        <v>45230.48312577546</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -779,129 +727,129 @@
         <v>24</v>
       </c>
       <c r="F37" s="1">
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="G37" s="1">
-        <v>7500</v>
+        <v>10500</v>
       </c>
       <c r="H37" s="3">
-        <v>45230.51493697916</v>
+        <v>45230.51429846065</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F38" s="1">
-        <v>1750</v>
+        <v>0</v>
       </c>
       <c r="G38" s="1">
-        <v>5250</v>
+        <v>7500</v>
       </c>
       <c r="H38" s="3">
-        <v>45230.517359826394</v>
+        <v>45230.51480040509</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F39" s="1">
-        <v>1875</v>
+        <v>0</v>
       </c>
       <c r="G39" s="1">
-        <v>5625</v>
+        <v>7500</v>
       </c>
       <c r="H39" s="3">
-        <v>45230.526474178245</v>
+        <v>45230.51493697916</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F40" s="1">
-        <v>0</v>
+        <v>1750</v>
       </c>
       <c r="G40" s="1">
-        <v>9000</v>
+        <v>5250</v>
       </c>
       <c r="H40" s="3">
-        <v>45230.527110069444</v>
+        <v>45230.517359826394</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F41" s="1">
-        <v>0</v>
+        <v>1875</v>
       </c>
       <c r="G41" s="1">
-        <v>7000</v>
+        <v>5625</v>
       </c>
       <c r="H41" s="3">
-        <v>45230.545366770835</v>
+        <v>45230.526474178245</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>13</v>
@@ -915,7 +863,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -927,39 +875,39 @@
         <v>0</v>
       </c>
       <c r="G42" s="1">
-        <v>7000</v>
+        <v>9000</v>
       </c>
       <c r="H42" s="3">
-        <v>45230.556492442134</v>
+        <v>45230.527110069444</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F43" s="1">
-        <v>2250</v>
+        <v>0</v>
       </c>
       <c r="G43" s="1">
-        <v>6750</v>
+        <v>7000</v>
       </c>
       <c r="H43" s="3">
-        <v>45230.56057988426</v>
+        <v>45230.545366770835</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>13</v>
@@ -973,80 +921,80 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="F44" s="1">
-        <v>1875</v>
+        <v>0</v>
       </c>
       <c r="G44" s="1">
-        <v>5625</v>
+        <v>7000</v>
       </c>
       <c r="H44" s="3">
-        <v>45230.575472627315</v>
+        <v>45230.556492442134</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="F45" s="1">
-        <v>0</v>
+        <v>2250</v>
       </c>
       <c r="G45" s="1">
-        <v>14000</v>
+        <v>6750</v>
       </c>
       <c r="H45" s="3">
-        <v>45231.41486247686</v>
+        <v>45230.56057988426</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="F46" s="1">
-        <v>0</v>
+        <v>1875</v>
       </c>
       <c r="G46" s="1">
-        <v>7500</v>
+        <v>5625</v>
       </c>
       <c r="H46" s="3">
-        <v>45231.41499884259</v>
+        <v>45230.575472627315</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>13</v>
@@ -1060,28 +1008,28 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F47" s="1">
-        <v>2250</v>
+        <v>0</v>
       </c>
       <c r="G47" s="1">
-        <v>6750</v>
+        <v>14000</v>
       </c>
       <c r="H47" s="3">
-        <v>45231.75643605324</v>
+        <v>45231.41486247686</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>18</v>
@@ -1089,57 +1037,57 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F48" s="1">
         <v>0</v>
       </c>
       <c r="G48" s="1">
-        <v>16000</v>
+        <v>7500</v>
       </c>
       <c r="H48" s="3">
-        <v>45231.765910428236</v>
+        <v>45231.41499884259</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F49" s="1">
-        <v>0</v>
+        <v>2250</v>
       </c>
       <c r="G49" s="1">
-        <v>7000</v>
+        <v>6750</v>
       </c>
       <c r="H49" s="3">
-        <v>45232.25594048611</v>
+        <v>45231.75643605324</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>18</v>
@@ -1147,22 +1095,22 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F50" s="1">
         <v>0</v>
       </c>
       <c r="G50" s="1">
-        <v>7500</v>
+        <v>16000</v>
       </c>
       <c r="H50" s="3">
-        <v>45232.256089849536</v>
+        <v>45231.765910428236</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>13</v>
@@ -1176,7 +1124,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1188,10 +1136,10 @@
         <v>0</v>
       </c>
       <c r="G51" s="1">
-        <v>9000</v>
+        <v>7000</v>
       </c>
       <c r="H51" s="3">
-        <v>45232.2562494213</v>
+        <v>45232.25594048611</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>13</v>
@@ -1205,7 +1153,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1217,10 +1165,10 @@
         <v>0</v>
       </c>
       <c r="G52" s="1">
-        <v>7000</v>
+        <v>7500</v>
       </c>
       <c r="H52" s="3">
-        <v>45232.25644429398</v>
+        <v>45232.256089849536</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>13</v>
@@ -1234,7 +1182,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1246,10 +1194,10 @@
         <v>0</v>
       </c>
       <c r="G53" s="1">
-        <v>10500</v>
+        <v>9000</v>
       </c>
       <c r="H53" s="3">
-        <v>45232.256622326386</v>
+        <v>45232.2562494213</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>13</v>
@@ -1263,7 +1211,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1275,10 +1223,10 @@
         <v>0</v>
       </c>
       <c r="G54" s="1">
-        <v>10500</v>
+        <v>7000</v>
       </c>
       <c r="H54" s="3">
-        <v>45232.25677541667</v>
+        <v>45232.25644429398</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>13</v>
@@ -1292,7 +1240,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1304,24 +1252,24 @@
         <v>0</v>
       </c>
       <c r="G55" s="1">
-        <v>9000</v>
+        <v>10500</v>
       </c>
       <c r="H55" s="3">
-        <v>45232.26625045139</v>
+        <v>45232.256622326386</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1333,24 +1281,24 @@
         <v>0</v>
       </c>
       <c r="G56" s="1">
-        <v>36000</v>
+        <v>10500</v>
       </c>
       <c r="H56" s="3">
-        <v>45232.266521377314</v>
+        <v>45232.25677541667</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1362,10 +1310,10 @@
         <v>0</v>
       </c>
       <c r="G57" s="1">
-        <v>234000</v>
+        <v>9000</v>
       </c>
       <c r="H57" s="3">
-        <v>45232.26717273148</v>
+        <v>45232.26625045139</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>20</v>
@@ -1375,6 +1323,122 @@
       </c>
       <c r="K57" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0</v>
+      </c>
+      <c r="G58" s="1">
+        <v>36000</v>
+      </c>
+      <c r="H58" s="3">
+        <v>45232.266521377314</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0</v>
+      </c>
+      <c r="G59" s="1">
+        <v>234000</v>
+      </c>
+      <c r="H59" s="3">
+        <v>45232.26717273148</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="1">
+        <v>0</v>
+      </c>
+      <c r="G60" s="1">
+        <v>22500</v>
+      </c>
+      <c r="H60" s="3">
+        <v>45233.50763043981</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="1">
+        <v>2250</v>
+      </c>
+      <c r="G61" s="1">
+        <v>6750</v>
+      </c>
+      <c r="H61" s="3">
+        <v>45234.547509525466</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>